<commit_message>
lead fuplicate not allowed
</commit_message>
<xml_diff>
--- a/public/assets/bimport.xlsx
+++ b/public/assets/bimport.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>First name</t>
   </si>
@@ -34,31 +34,52 @@
     <t>Lead Subject</t>
   </si>
   <si>
-    <t>Arun</t>
-  </si>
-  <si>
-    <t>Kumar</t>
-  </si>
-  <si>
-    <t>arunk@yopmail.com</t>
-  </si>
-  <si>
-    <t>Chennai</t>
-  </si>
-  <si>
-    <t>Enquiry Online</t>
-  </si>
-  <si>
-    <t>ArunKevin</t>
-  </si>
-  <si>
-    <t>kevin</t>
-  </si>
-  <si>
-    <t>kevin@yopmail.com</t>
-  </si>
-  <si>
-    <t>Ambattur, chennai</t>
+    <t>Offer</t>
+  </si>
+  <si>
+    <t>Arumbakkam</t>
+  </si>
+  <si>
+    <t>Guindy</t>
+  </si>
+  <si>
+    <t>Of Sale</t>
+  </si>
+  <si>
+    <t>Lead Stage</t>
+  </si>
+  <si>
+    <t>Lead Source</t>
+  </si>
+  <si>
+    <t>Interested</t>
+  </si>
+  <si>
+    <t>Not Interested</t>
+  </si>
+  <si>
+    <t>Facebook</t>
+  </si>
+  <si>
+    <t>Linkedin</t>
+  </si>
+  <si>
+    <t>rajendran</t>
+  </si>
+  <si>
+    <t>kumar</t>
+  </si>
+  <si>
+    <t>rajendran@yopmail.com</t>
+  </si>
+  <si>
+    <t>Oliya</t>
+  </si>
+  <si>
+    <t>Ov</t>
+  </si>
+  <si>
+    <t>olioo@yopmail.com</t>
   </si>
 </sst>
 </file>
@@ -91,14 +112,15 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0563C1"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
@@ -120,21 +142,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -348,10 +372,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -362,7 +386,7 @@
     <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -381,42 +405,63 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="4">
+        <v>8528528522</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="4">
+        <v>7417417411</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="5">
-        <v>9551702545</v>
-      </c>
-      <c r="E2" s="6" t="s">
+      <c r="F3" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="G3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="5">
-        <v>7551201230</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>14</v>
+      <c r="H3" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>